<commit_message>
DB Patch applied - 18th Sep
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +61,18 @@
   </si>
   <si>
     <t>EKA_METALS_PATCH_0137.txt</t>
+  </si>
+  <si>
+    <t>CDC Patch to be released:</t>
+  </si>
+  <si>
+    <t>EKA_CDC_1.0_Objects _0008.sql</t>
+  </si>
+  <si>
+    <t>EKA_CDC_1.0_Objects _0007.sql</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0145.txt</t>
   </si>
 </sst>
 </file>
@@ -393,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,7 +498,28 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="1"/>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40804</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Patch status as on 30th Sep
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -63,16 +63,22 @@
     <t>EKA_METALS_PATCH_0137.txt</t>
   </si>
   <si>
-    <t>CDC Patch to be released:</t>
-  </si>
-  <si>
-    <t>EKA_CDC_1.0_Objects _0008.sql</t>
-  </si>
-  <si>
-    <t>EKA_CDC_1.0_Objects _0007.sql</t>
-  </si>
-  <si>
     <t>EKA_METALS_PATCH_0145.txt</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0147.txt</t>
+  </si>
+  <si>
+    <t>1.4.5</t>
+  </si>
+  <si>
+    <t>EKA_CDC_1.3.2_Patch_0053.txt</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0155.txt</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0167.txt</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,20 +511,63 @@
         <v>40804</v>
       </c>
       <c r="I4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40807</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="D12" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>40810</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40814</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>40816</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Patches applied as on 24th Nov
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>CDC 1.3.3</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0214.txt</t>
+  </si>
+  <si>
+    <t>1.4.9</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0234.txt</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0237.txt</t>
   </si>
 </sst>
 </file>
@@ -427,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="32.42578125" customWidth="1"/>
@@ -627,6 +639,39 @@
       </c>
       <c r="I10" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="1">
+        <v>40862</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="2">
+        <v>40870</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="2">
+        <v>40871</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with 20th dec status
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>EKA_METALS_PATCH_0261.txt</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0289</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0283</t>
   </si>
 </sst>
 </file>
@@ -454,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,6 +728,22 @@
       </c>
       <c r="I17" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="2">
+        <v>40893</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="2">
+        <v>40897</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB Patch applied as of 9th Feb
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>EKA_METALS_PATCH_0355</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0357</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0382</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -881,6 +887,27 @@
       </c>
       <c r="I32" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="2">
+        <v>40938</v>
+      </c>
+      <c r="I33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="2">
+        <v>40939</v>
+      </c>
+      <c r="I34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="2">
+        <v>40948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated status as on 10th April
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -253,6 +253,27 @@
   </si>
   <si>
     <t>EKA_METALS_PATCH_0613</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0617</t>
+  </si>
+  <si>
+    <t>Released TO QA for UAT</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0650</t>
+  </si>
+  <si>
+    <t>Applied to Ref(METAL_APP_REF)</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0655</t>
+  </si>
+  <si>
+    <t>Applied To Blank</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0665</t>
   </si>
 </sst>
 </file>
@@ -268,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -278,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,12 +321,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1146,7 +1174,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
+    <row r="49" spans="2:13">
       <c r="B49" s="2">
         <v>40977</v>
       </c>
@@ -1157,7 +1185,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:13">
       <c r="B50" s="2">
         <v>40982</v>
       </c>
@@ -1168,7 +1196,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
+    <row r="51" spans="2:13">
       <c r="B51" s="2">
         <v>40983</v>
       </c>
@@ -1179,7 +1207,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="2:11">
+    <row r="52" spans="2:13">
       <c r="B52" s="2">
         <v>40984</v>
       </c>
@@ -1190,7 +1218,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="53" spans="2:11">
+    <row r="53" spans="2:13">
       <c r="B53" s="2">
         <v>40988</v>
       </c>
@@ -1204,7 +1232,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="2:11">
+    <row r="54" spans="2:13">
       <c r="B54" s="2">
         <v>40988</v>
       </c>
@@ -1215,7 +1243,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
+    <row r="55" spans="2:13">
       <c r="B55" s="2">
         <v>40989</v>
       </c>
@@ -1226,7 +1254,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="2:11">
+    <row r="56" spans="2:13">
       <c r="B56" s="2">
         <v>40993</v>
       </c>
@@ -1237,9 +1265,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="2:11">
+    <row r="57" spans="2:13">
       <c r="B57" s="2">
-        <v>40993</v>
+        <v>40995</v>
       </c>
       <c r="I57" t="s">
         <v>76</v>
@@ -1251,7 +1279,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="2:11">
+    <row r="58" spans="2:13">
       <c r="B58" s="2">
         <v>40996</v>
       </c>
@@ -1262,12 +1290,80 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
+    <row r="59" spans="2:13">
+      <c r="B59" s="2">
+        <v>40997</v>
+      </c>
       <c r="I59" t="s">
         <v>78</v>
       </c>
       <c r="J59" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13">
+      <c r="B60" s="2">
+        <v>40998</v>
+      </c>
+      <c r="I60" t="s">
+        <v>79</v>
+      </c>
+      <c r="J60" t="s">
+        <v>62</v>
+      </c>
+      <c r="K60" t="s">
+        <v>80</v>
+      </c>
+      <c r="M60" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13">
+      <c r="B61" s="2">
+        <v>41003</v>
+      </c>
+      <c r="I61" t="s">
+        <v>81</v>
+      </c>
+      <c r="J61" t="s">
+        <v>82</v>
+      </c>
+      <c r="K61" t="s">
+        <v>80</v>
+      </c>
+      <c r="M61" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13">
+      <c r="B62" s="2">
+        <v>41004</v>
+      </c>
+      <c r="I62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J62" t="s">
+        <v>82</v>
+      </c>
+      <c r="K62" t="s">
+        <v>80</v>
+      </c>
+      <c r="M62" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13">
+      <c r="B63" s="2">
+        <v>41009</v>
+      </c>
+      <c r="I63" t="s">
+        <v>85</v>
+      </c>
+      <c r="J63" t="s">
+        <v>82</v>
+      </c>
+      <c r="M63" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with 23rd Release.
</commit_message>
<xml_diff>
--- a/DB Patch Applied.xlsx
+++ b/DB Patch Applied.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="89">
   <si>
     <t>Date</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>EKA_METALS_PATCH_0665</t>
+  </si>
+  <si>
+    <t>Applied to Ref(METALS_MAIN_APP_REF@CHMDB)</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0700</t>
+  </si>
+  <si>
+    <t>EKA_METALS_PATCH_0704</t>
   </si>
 </sst>
 </file>
@@ -622,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1362,8 +1371,33 @@
       <c r="J63" t="s">
         <v>82</v>
       </c>
+      <c r="K63" t="s">
+        <v>60</v>
+      </c>
       <c r="M63" s="5" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13">
+      <c r="B64" s="2">
+        <v>41019</v>
+      </c>
+      <c r="I64" t="s">
+        <v>87</v>
+      </c>
+      <c r="J64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="2">
+        <v>41022</v>
+      </c>
+      <c r="I65" t="s">
+        <v>88</v>
+      </c>
+      <c r="J65" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>